<commit_message>
Update SDI input data to just have country values
</commit_message>
<xml_diff>
--- a/data-raw/ihme_sdi_gbd_2019.xlsx
+++ b/data-raw/ihme_sdi_gbd_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caldwellst/Documents/repos/packages/billionaiRe/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6CF9DE-5391-BB46-8249-BD93DEC87D2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2A5573-2F8A-444A-9611-02485B64667A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3691,8 +3691,8 @@
   </sheetPr>
   <dimension ref="A1:AE207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>